<commit_message>
update on 15 nov
</commit_message>
<xml_diff>
--- a/Learning/options_made_easy.xlsx
+++ b/Learning/options_made_easy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Finance\stock_automata\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Finance\stock_automata\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F096DC83-6E63-452F-A01D-09B79CFA5047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4029EDE-8613-4513-895B-740A692969CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A54D7702-EB53-4A3C-9FDB-BB1FDCB5F0D9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>Strike price</t>
   </si>
@@ -156,6 +156,78 @@
   </si>
   <si>
     <t>!&lt;0.5</t>
+  </si>
+  <si>
+    <t>GAMMA</t>
+  </si>
+  <si>
+    <t>gamma tells how much delta will change when stock price  changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delta is speed and gamma is acceltrator </t>
+  </si>
+  <si>
+    <t>ATM has highest Gamma</t>
+  </si>
+  <si>
+    <t>gamma increase to close of expiration</t>
+  </si>
+  <si>
+    <t>THETA</t>
+  </si>
+  <si>
+    <t>mtm</t>
+  </si>
+  <si>
+    <t>time decays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at expiry theta reaches to 0 </t>
+  </si>
+  <si>
+    <t>ATM has the highest theta</t>
+  </si>
+  <si>
+    <t>VEGA</t>
+  </si>
+  <si>
+    <t>volatitllity</t>
+  </si>
+  <si>
+    <t>valatility make large part of extrinsic value</t>
+  </si>
+  <si>
+    <t>buy option at low volatility</t>
+  </si>
+  <si>
+    <t>sell option at high volatility</t>
+  </si>
+  <si>
+    <t>neg-ve for buy and +ve for sale</t>
+  </si>
+  <si>
+    <t>implied volitility</t>
+  </si>
+  <si>
+    <t>india vix is IV</t>
+  </si>
+  <si>
+    <t>Stretegies</t>
+  </si>
+  <si>
+    <t>1. long call</t>
+  </si>
+  <si>
+    <t>2. sell  put</t>
+  </si>
+  <si>
+    <t>don’t buy on high IV</t>
+  </si>
+  <si>
+    <t>don’t sell on market crash</t>
+  </si>
+  <si>
+    <t>3. Bull call spread</t>
   </si>
 </sst>
 </file>
@@ -525,7 +597,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -533,16 +605,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70DEED42-6234-4008-B5E0-5FB45374C6CB}">
-  <dimension ref="A2:F36"/>
+  <dimension ref="A2:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -796,7 +869,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="3" t="s">
         <v>33</v>
@@ -805,7 +878,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>3</v>
       </c>
@@ -815,8 +888,11 @@
       <c r="D34" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
@@ -827,7 +903,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>1</v>
       </c>
@@ -836,6 +912,111 @@
       </c>
       <c r="D36" s="2" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>